<commit_message>
unified snp masking/filtering in alignment and direct mode
</commit_message>
<xml_diff>
--- a/ddprimer/test_data/Primers/Primers_fasta1_vs_fasta2.xlsx
+++ b/ddprimer/test_data/Primers/Primers_fasta1_vs_fasta2.xlsx
@@ -80,7 +80,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -100,9 +100,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB16"/>
+  <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -887,22 +884,22 @@
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>XSP1</t>
+          <t>PDH-E1 ALPHA</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>CTACGACATGGACGACATC</t>
+          <t>CAGTAACCTTGCCGAAGAG</t>
         </is>
       </c>
       <c r="C5" s="6" t="n">
-        <v>57.44369071181501</v>
+        <v>57.85284621491923</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>1.1220987618692</v>
+        <v>1.418635688603434</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-0.3097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>0.007</v>
@@ -912,14 +909,14 @@
       </c>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>GACAATGGAGGAACAGCTC</t>
+          <t>GCTCCTTACCAAGTCTGAC</t>
         </is>
       </c>
       <c r="I5" s="6" t="n">
-        <v>57.83082272420569</v>
+        <v>57.15171809660262</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>1.396612197889898</v>
+        <v>1.414071377081587</v>
       </c>
       <c r="K5" s="6" t="n">
         <v>0</v>
@@ -928,24 +925,24 @@
         <v>0.007</v>
       </c>
       <c r="M5" s="6" t="n">
-        <v>1.1</v>
+        <v>3.7</v>
       </c>
       <c r="N5" s="6" t="n">
-        <v>2.518710959759098</v>
+        <v>2.832707065685021</v>
       </c>
       <c r="O5" s="7" t="inlineStr">
         <is>
-          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
+          <t>CCGTGACCATGTCCATGCCCTCAGCA</t>
         </is>
       </c>
       <c r="P5" s="6" t="n">
-        <v>64.22598535419934</v>
+        <v>64.46575342767647</v>
       </c>
       <c r="Q5" s="6" t="n">
-        <v>6.774014645800662</v>
+        <v>6.534246572323525</v>
       </c>
       <c r="R5" s="6" t="n">
-        <v>-0.7341697216033936</v>
+        <v>-0.8420321941375732</v>
       </c>
       <c r="S5" s="6" t="n">
         <v>1.51e-06</v>
@@ -955,73 +952,73 @@
       </c>
       <c r="U5" s="7" t="inlineStr">
         <is>
-          <t>CTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCC</t>
+          <t>CAGTAACCTTGCCGAAGAGCTCGCTCATAACAGCACGAGCAGAGACACCTTTGCTGAGGGCATGGACATGGTCACGGTAGGTACTAACGACAGAGTCAGACTTGGTAAGGAGCT</t>
         </is>
       </c>
       <c r="V5" s="6" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="W5" s="6" t="n">
-        <v>53.98230088495575</v>
+        <v>52.63157894736842</v>
       </c>
       <c r="X5" s="6" t="n">
-        <v>-6.521465301513672</v>
+        <v>-8.800433158874512</v>
       </c>
       <c r="Y5" s="6" t="inlineStr">
         <is>
-          <t>CP002687.1</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="Z5" s="6" t="inlineStr">
         <is>
-          <t>96840</t>
+          <t>48586</t>
         </is>
       </c>
       <c r="AA5" s="6" t="inlineStr">
         <is>
-          <t>LR699773.1</t>
+          <t>LR699770.1</t>
         </is>
       </c>
       <c r="AB5" s="6" t="n">
-        <v>149749</v>
+        <v>47493</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>XSP1</t>
+          <t>PDH-E1 ALPHA</t>
         </is>
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>CTGGCTTAGTCTACGACATG</t>
+          <t>CGAAGAGCTCGCTCATAAC</t>
         </is>
       </c>
       <c r="C6" s="6" t="n">
-        <v>57.6139686963578</v>
+        <v>58.11854570998298</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>1.363968696357801</v>
+        <v>1.684335183667191</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>0</v>
+        <v>-0.8030736446380615</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
-          <t>AGGGACAATGGAGGAACAG</t>
+          <t>ACCAAGTCTGACTCTGTCG</t>
         </is>
       </c>
       <c r="I6" s="6" t="n">
-        <v>58.60725372965351</v>
+        <v>58.65308273860558</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v>2.173043203337716</v>
+        <v>2.218872212289785</v>
       </c>
       <c r="K6" s="6" t="n">
         <v>0</v>
@@ -1030,24 +1027,24 @@
         <v>0.007</v>
       </c>
       <c r="M6" s="6" t="n">
-        <v>1.1</v>
+        <v>3.7</v>
       </c>
       <c r="N6" s="6" t="n">
-        <v>3.537011899695518</v>
+        <v>3.903207395956976</v>
       </c>
       <c r="O6" s="7" t="inlineStr">
         <is>
-          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
+          <t>CCGTGACCATGTCCATGCCCTCAGCA</t>
         </is>
       </c>
       <c r="P6" s="6" t="n">
-        <v>64.22598535419934</v>
+        <v>64.46575342767647</v>
       </c>
       <c r="Q6" s="6" t="n">
-        <v>6.774014645800662</v>
+        <v>6.534246572323525</v>
       </c>
       <c r="R6" s="6" t="n">
-        <v>-0.7341697216033936</v>
+        <v>-0.8420321941375732</v>
       </c>
       <c r="S6" s="6" t="n">
         <v>1.51e-06</v>
@@ -1057,175 +1054,173 @@
       </c>
       <c r="U6" s="7" t="inlineStr">
         <is>
-          <t>CTGGCTTAGTCTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCCCTG</t>
+          <t>CGAAGAGCTCGCTCATAACAGCACGAGCAGAGACACCTTTGCTGAGGGCATGGACATGGTCACGGTAGGTACTAACGACAGAGTCAGACTTGGTA</t>
         </is>
       </c>
       <c r="V6" s="6" t="n">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="W6" s="6" t="n">
-        <v>53.96825396825397</v>
+        <v>52.63157894736842</v>
       </c>
       <c r="X6" s="6" t="n">
-        <v>-6.521465301513672</v>
+        <v>-8.800433158874512</v>
       </c>
       <c r="Y6" s="6" t="inlineStr">
         <is>
-          <t>CP002687.1</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="Z6" s="6" t="inlineStr">
         <is>
-          <t>96830</t>
+          <t>48598</t>
         </is>
       </c>
       <c r="AA6" s="6" t="inlineStr">
         <is>
-          <t>LR699773.1</t>
+          <t>LR699770.1</t>
         </is>
       </c>
       <c r="AB6" s="6" t="n">
-        <v>149739</v>
+        <v>47505</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>XSP1</t>
+          <t>CYP703A2</t>
         </is>
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>CCCAACAATCCAACTCACG</t>
+          <t>GAACGATCCCGATACCATC</t>
         </is>
       </c>
       <c r="C7" s="6" t="n">
-        <v>58.74250943646473</v>
+        <v>57.18013716608459</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>2.308298910148938</v>
+        <v>1.385652307599617</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>0</v>
+        <v>-0.8097348213195801</v>
       </c>
       <c r="F7" s="6" t="n">
         <v>0.007</v>
       </c>
-      <c r="G7" s="6" t="n">
-        <v>3.7</v>
-      </c>
+      <c r="G7" s="6" t="inlineStr"/>
       <c r="H7" s="7" t="inlineStr">
         <is>
-          <t>CCACCACTTTGAAGCTTCTC</t>
+          <t>CACATCCATACGCTAGGTG</t>
         </is>
       </c>
       <c r="I7" s="6" t="n">
-        <v>58.87532172899461</v>
+        <v>57.40147050241876</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>2.625321728994606</v>
+        <v>1.164318971265448</v>
       </c>
       <c r="K7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v>0.3</v>
+        <v>3.7</v>
       </c>
       <c r="N7" s="6" t="n">
-        <v>4.933620639143545</v>
+        <v>2.549971278865065</v>
       </c>
       <c r="O7" s="7" t="inlineStr">
         <is>
-          <t>CCGCCACCGTCCGAGCACCG</t>
+          <t>TCGAGACCCAAAACACTCGCCGCAGT</t>
         </is>
       </c>
       <c r="P7" s="6" t="n">
-        <v>64.7335341111355</v>
+        <v>64.30135325099201</v>
       </c>
       <c r="Q7" s="6" t="n">
-        <v>0.2664658888645022</v>
+        <v>6.698646749007992</v>
       </c>
       <c r="R7" s="6" t="n">
-        <v>0</v>
+        <v>-1.419864654541016</v>
       </c>
       <c r="S7" s="6" t="n">
-        <v>0.002</v>
+        <v>1.51e-06</v>
       </c>
       <c r="T7" s="6" t="n">
-        <v>1.1</v>
+        <v>1.4</v>
       </c>
       <c r="U7" s="7" t="inlineStr">
         <is>
-          <t>CCCAACAATCCAACTCACGTTGAGATCCGCCAAAACGTCCACATTGGCTGTGTTCAGGCGGAGAGTCACCAACGTGGGACCACCGTCGTCGGTCTACACCGCCACCGTCCGAGCACCGAAAGGAGTAGAAATCACGGTGGAGCCACAGAGTTTGTCATTTTCAAAGGCTTCACAAAAGAGAAGCTTCAAAGTGGTGGT</t>
+          <t>GAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATGTGG</t>
         </is>
       </c>
       <c r="V7" s="6" t="n">
-        <v>197</v>
+        <v>101</v>
       </c>
       <c r="W7" s="6" t="n">
-        <v>53.03030303030303</v>
+        <v>51.9607843137255</v>
       </c>
       <c r="X7" s="6" t="n">
-        <v>-17.26604652404785</v>
+        <v>-5.947404861450195</v>
       </c>
       <c r="Y7" s="6" t="inlineStr">
         <is>
-          <t>CP002687.1</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="Z7" s="6" t="inlineStr">
         <is>
-          <t>96981</t>
+          <t>112527</t>
         </is>
       </c>
       <c r="AA7" s="6" t="inlineStr">
         <is>
-          <t>LR699773.1</t>
+          <t>LR699770.1</t>
         </is>
       </c>
       <c r="AB7" s="6" t="n">
-        <v>149890</v>
+        <v>111452</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>PDH-E1 ALPHA</t>
+          <t>CYP703A2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>CAGTAACCTTGCCGAAGAG</t>
+          <t>CAACGAACGATCCCGATAC</t>
         </is>
       </c>
       <c r="C8" s="6" t="n">
-        <v>57.85284621491923</v>
+        <v>58.1158368244387</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>1.418635688603434</v>
+        <v>1.681626298122911</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>0</v>
+        <v>-0.8097348213195801</v>
       </c>
       <c r="F8" s="6" t="n">
         <v>0.007</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>1.1</v>
+        <v>3.7</v>
       </c>
       <c r="H8" s="7" t="inlineStr">
         <is>
-          <t>GCTCCTTACCAAGTCTGAC</t>
+          <t>ATCCATACGCTAGGTGGAC</t>
         </is>
       </c>
       <c r="I8" s="6" t="n">
-        <v>57.15171809660262</v>
+        <v>58.25082796726878</v>
       </c>
       <c r="J8" s="6" t="n">
-        <v>1.414071377081587</v>
+        <v>1.816617440952985</v>
       </c>
       <c r="K8" s="6" t="n">
         <v>0</v>
@@ -1234,44 +1229,44 @@
         <v>0.007</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="N8" s="6" t="n">
-        <v>2.832707065685021</v>
+        <v>3.498243739075896</v>
       </c>
       <c r="O8" s="7" t="inlineStr">
         <is>
-          <t>CCGTGACCATGTCCATGCCCTCAGCA</t>
+          <t>TCATCGAGACCCAAAACACTCGCCGCA</t>
         </is>
       </c>
       <c r="P8" s="6" t="n">
-        <v>64.46575342767647</v>
+        <v>64.20487603053124</v>
       </c>
       <c r="Q8" s="6" t="n">
-        <v>6.534246572323525</v>
+        <v>7.795123969468762</v>
       </c>
       <c r="R8" s="6" t="n">
-        <v>-0.8420321941375732</v>
+        <v>-1.419864654541016</v>
       </c>
       <c r="S8" s="6" t="n">
-        <v>1.51e-06</v>
+        <v>5.4e-07</v>
       </c>
       <c r="T8" s="6" t="n">
-        <v>1.4</v>
+        <v>0.042</v>
       </c>
       <c r="U8" s="7" t="inlineStr">
         <is>
-          <t>CAGTAACCTTGCCGAAGAGCTCGCTCATAACAGCACGAGCAGAGACACCTTTGCTGAGGGCATGGACATGGTCACGGTAGGTACTAACGACAGAGTCAGACTTGGTAAGGAGCT</t>
+          <t>CAACGAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATG</t>
         </is>
       </c>
       <c r="V8" s="6" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="W8" s="6" t="n">
-        <v>52.63157894736842</v>
+        <v>51.45631067961165</v>
       </c>
       <c r="X8" s="6" t="n">
-        <v>-8.800433158874512</v>
+        <v>-5.947404861450195</v>
       </c>
       <c r="Y8" s="6" t="inlineStr">
         <is>
@@ -1280,7 +1275,7 @@
       </c>
       <c r="Z8" s="6" t="inlineStr">
         <is>
-          <t>48586</t>
+          <t>112523</t>
         </is>
       </c>
       <c r="AA8" s="6" t="inlineStr">
@@ -1289,28 +1284,28 @@
         </is>
       </c>
       <c r="AB8" s="6" t="n">
-        <v>47493</v>
+        <v>111448</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>PDH-E1 ALPHA</t>
+          <t>XSP1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>CGAAGAGCTCGCTCATAAC</t>
+          <t>CTACGACATGGACGACATC</t>
         </is>
       </c>
       <c r="C9" s="6" t="n">
-        <v>58.11854570998298</v>
+        <v>57.44369071181501</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>1.684335183667191</v>
+        <v>1.1220987618692</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>-0.8030736446380615</v>
+        <v>-0.3097348213195801</v>
       </c>
       <c r="F9" s="6" t="n">
         <v>0.007</v>
@@ -1320,14 +1315,14 @@
       </c>
       <c r="H9" s="7" t="inlineStr">
         <is>
-          <t>ACCAAGTCTGACTCTGTCG</t>
+          <t>GACAATGGAGGAACAGCTC</t>
         </is>
       </c>
       <c r="I9" s="6" t="n">
-        <v>58.65308273860558</v>
+        <v>57.83082272420569</v>
       </c>
       <c r="J9" s="6" t="n">
-        <v>2.218872212289785</v>
+        <v>1.396612197889898</v>
       </c>
       <c r="K9" s="6" t="n">
         <v>0</v>
@@ -1336,24 +1331,24 @@
         <v>0.007</v>
       </c>
       <c r="M9" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="N9" s="6" t="n">
-        <v>3.903207395956976</v>
+        <v>2.518710959759098</v>
       </c>
       <c r="O9" s="7" t="inlineStr">
         <is>
-          <t>CCGTGACCATGTCCATGCCCTCAGCA</t>
+          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
         </is>
       </c>
       <c r="P9" s="6" t="n">
-        <v>64.46575342767647</v>
+        <v>64.22598535419934</v>
       </c>
       <c r="Q9" s="6" t="n">
-        <v>6.534246572323525</v>
+        <v>6.774014645800662</v>
       </c>
       <c r="R9" s="6" t="n">
-        <v>-0.8420321941375732</v>
+        <v>-0.7341697216033936</v>
       </c>
       <c r="S9" s="6" t="n">
         <v>1.51e-06</v>
@@ -1363,71 +1358,73 @@
       </c>
       <c r="U9" s="7" t="inlineStr">
         <is>
-          <t>CGAAGAGCTCGCTCATAACAGCACGAGCAGAGACACCTTTGCTGAGGGCATGGACATGGTCACGGTAGGTACTAACGACAGAGTCAGACTTGGTA</t>
+          <t>CTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCC</t>
         </is>
       </c>
       <c r="V9" s="6" t="n">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="W9" s="6" t="n">
-        <v>52.63157894736842</v>
+        <v>53.98230088495575</v>
       </c>
       <c r="X9" s="6" t="n">
-        <v>-8.800433158874512</v>
+        <v>-6.521465301513672</v>
       </c>
       <c r="Y9" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>CP002687.1</t>
         </is>
       </c>
       <c r="Z9" s="6" t="inlineStr">
         <is>
-          <t>48598</t>
+          <t>96840</t>
         </is>
       </c>
       <c r="AA9" s="6" t="inlineStr">
         <is>
-          <t>LR699770.1</t>
+          <t>LR699773.1</t>
         </is>
       </c>
       <c r="AB9" s="6" t="n">
-        <v>47505</v>
+        <v>149749</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>CYP703A2</t>
+          <t>XSP1</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>GAACGATCCCGATACCATC</t>
+          <t>CTGGCTTAGTCTACGACATG</t>
         </is>
       </c>
       <c r="C10" s="6" t="n">
-        <v>57.18013716608459</v>
+        <v>57.6139686963578</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>1.385652307599617</v>
+        <v>1.363968696357801</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F10" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="G10" s="6" t="inlineStr"/>
+        <v>0.002</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>3.7</v>
+      </c>
       <c r="H10" s="7" t="inlineStr">
         <is>
-          <t>CACATCCATACGCTAGGTG</t>
+          <t>AGGGACAATGGAGGAACAG</t>
         </is>
       </c>
       <c r="I10" s="6" t="n">
-        <v>57.40147050241876</v>
+        <v>58.60725372965351</v>
       </c>
       <c r="J10" s="6" t="n">
-        <v>1.164318971265448</v>
+        <v>2.173043203337716</v>
       </c>
       <c r="K10" s="6" t="n">
         <v>0</v>
@@ -1436,24 +1433,24 @@
         <v>0.007</v>
       </c>
       <c r="M10" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="N10" s="6" t="n">
-        <v>2.549971278865065</v>
+        <v>3.537011899695518</v>
       </c>
       <c r="O10" s="7" t="inlineStr">
         <is>
-          <t>TCGAGACCCAAAACACTCGCCGCAGT</t>
+          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
         </is>
       </c>
       <c r="P10" s="6" t="n">
-        <v>64.30135325099201</v>
+        <v>64.22598535419934</v>
       </c>
       <c r="Q10" s="6" t="n">
-        <v>6.698646749007992</v>
+        <v>6.774014645800662</v>
       </c>
       <c r="R10" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>-0.7341697216033936</v>
       </c>
       <c r="S10" s="6" t="n">
         <v>1.51e-06</v>
@@ -1463,56 +1460,56 @@
       </c>
       <c r="U10" s="7" t="inlineStr">
         <is>
-          <t>GAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATGTGG</t>
+          <t>CTGGCTTAGTCTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCCCTG</t>
         </is>
       </c>
       <c r="V10" s="6" t="n">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="W10" s="6" t="n">
-        <v>51.9607843137255</v>
+        <v>53.96825396825397</v>
       </c>
       <c r="X10" s="6" t="n">
-        <v>-5.947404861450195</v>
+        <v>-6.521465301513672</v>
       </c>
       <c r="Y10" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>CP002687.1</t>
         </is>
       </c>
       <c r="Z10" s="6" t="inlineStr">
         <is>
-          <t>112527</t>
+          <t>96830</t>
         </is>
       </c>
       <c r="AA10" s="6" t="inlineStr">
         <is>
-          <t>LR699770.1</t>
+          <t>LR699773.1</t>
         </is>
       </c>
       <c r="AB10" s="6" t="n">
-        <v>111452</v>
+        <v>149739</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>CYP703A2</t>
+          <t>XSP1</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>CAACGAACGATCCCGATAC</t>
+          <t>CCCAACAATCCAACTCACG</t>
         </is>
       </c>
       <c r="C11" s="6" t="n">
-        <v>58.1158368244387</v>
+        <v>58.74250943646473</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>1.681626298122911</v>
+        <v>2.308298910148938</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F11" s="6" t="n">
         <v>0.007</v>
@@ -1522,269 +1519,79 @@
       </c>
       <c r="H11" s="7" t="inlineStr">
         <is>
-          <t>ATCCATACGCTAGGTGGAC</t>
+          <t>CCACCACTTTGAAGCTTCTC</t>
         </is>
       </c>
       <c r="I11" s="6" t="n">
-        <v>58.25082796726878</v>
+        <v>58.87532172899461</v>
       </c>
       <c r="J11" s="6" t="n">
-        <v>1.816617440952985</v>
+        <v>2.625321728994606</v>
       </c>
       <c r="K11" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="M11" s="6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="N11" s="6" t="n">
+        <v>4.933620639143545</v>
+      </c>
+      <c r="O11" s="7" t="inlineStr">
+        <is>
+          <t>CCGCCACCGTCCGAGCACCG</t>
+        </is>
+      </c>
+      <c r="P11" s="6" t="n">
+        <v>64.7335341111355</v>
+      </c>
+      <c r="Q11" s="6" t="n">
+        <v>0.2664658888645022</v>
+      </c>
+      <c r="R11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="T11" s="6" t="n">
         <v>1.1</v>
       </c>
-      <c r="N11" s="6" t="n">
-        <v>3.498243739075896</v>
-      </c>
-      <c r="O11" s="7" t="inlineStr">
-        <is>
-          <t>TCATCGAGACCCAAAACACTCGCCGCA</t>
-        </is>
-      </c>
-      <c r="P11" s="6" t="n">
-        <v>64.20487603053124</v>
-      </c>
-      <c r="Q11" s="6" t="n">
-        <v>7.795123969468762</v>
-      </c>
-      <c r="R11" s="6" t="n">
-        <v>-1.419864654541016</v>
-      </c>
-      <c r="S11" s="6" t="n">
-        <v>5.4e-07</v>
-      </c>
-      <c r="T11" s="6" t="n">
-        <v>0.042</v>
-      </c>
       <c r="U11" s="7" t="inlineStr">
         <is>
-          <t>CAACGAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATG</t>
+          <t>CCCAACAATCCAACTCACGTTGAGATCCGCCAAAACGTCCACATTGGCTGTGTTCAGGCGGAGAGTCACCAACGTGGGACCACCGTCGTCGGTCTACACCGCCACCGTCCGAGCACCGAAAGGAGTAGAAATCACGGTGGAGCCACAGAGTTTGTCATTTTCAAAGGCTTCACAAAAGAGAAGCTTCAAAGTGGTGGT</t>
         </is>
       </c>
       <c r="V11" s="6" t="n">
-        <v>102</v>
+        <v>197</v>
       </c>
       <c r="W11" s="6" t="n">
-        <v>51.45631067961165</v>
+        <v>53.03030303030303</v>
       </c>
       <c r="X11" s="6" t="n">
-        <v>-5.947404861450195</v>
+        <v>-17.26604652404785</v>
       </c>
       <c r="Y11" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>CP002687.1</t>
         </is>
       </c>
       <c r="Z11" s="6" t="inlineStr">
         <is>
-          <t>112523</t>
+          <t>96981</t>
         </is>
       </c>
       <c r="AA11" s="6" t="inlineStr">
         <is>
-          <t>LR699770.1</t>
+          <t>LR699773.1</t>
         </is>
       </c>
       <c r="AB11" s="6" t="n">
-        <v>111448</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>CP002688.1</t>
-        </is>
-      </c>
-      <c r="B12" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C12" s="6" t="inlineStr"/>
-      <c r="D12" s="6" t="inlineStr"/>
-      <c r="E12" s="6" t="inlineStr"/>
-      <c r="F12" s="6" t="inlineStr"/>
-      <c r="G12" s="6" t="inlineStr"/>
-      <c r="H12" s="7" t="inlineStr"/>
-      <c r="I12" s="6" t="inlineStr"/>
-      <c r="J12" s="6" t="inlineStr"/>
-      <c r="K12" s="6" t="inlineStr"/>
-      <c r="L12" s="6" t="inlineStr"/>
-      <c r="M12" s="6" t="inlineStr"/>
-      <c r="N12" s="6" t="inlineStr"/>
-      <c r="O12" s="7" t="inlineStr"/>
-      <c r="P12" s="6" t="inlineStr"/>
-      <c r="Q12" s="6" t="inlineStr"/>
-      <c r="R12" s="6" t="inlineStr"/>
-      <c r="S12" s="6" t="inlineStr"/>
-      <c r="T12" s="6" t="inlineStr"/>
-      <c r="U12" s="7" t="inlineStr"/>
-      <c r="V12" s="6" t="inlineStr"/>
-      <c r="W12" s="6" t="inlineStr"/>
-      <c r="X12" s="6" t="inlineStr"/>
-      <c r="Y12" s="6" t="inlineStr"/>
-      <c r="Z12" s="6" t="inlineStr"/>
-      <c r="AA12" s="6" t="inlineStr"/>
-      <c r="AB12" s="6" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="inlineStr">
-        <is>
-          <t>CP002686.1</t>
-        </is>
-      </c>
-      <c r="B13" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C13" s="6" t="inlineStr"/>
-      <c r="D13" s="6" t="inlineStr"/>
-      <c r="E13" s="6" t="inlineStr"/>
-      <c r="F13" s="6" t="inlineStr"/>
-      <c r="G13" s="6" t="inlineStr"/>
-      <c r="H13" s="7" t="inlineStr"/>
-      <c r="I13" s="6" t="inlineStr"/>
-      <c r="J13" s="6" t="inlineStr"/>
-      <c r="K13" s="6" t="inlineStr"/>
-      <c r="L13" s="6" t="inlineStr"/>
-      <c r="M13" s="6" t="inlineStr"/>
-      <c r="N13" s="6" t="inlineStr"/>
-      <c r="O13" s="7" t="inlineStr"/>
-      <c r="P13" s="6" t="inlineStr"/>
-      <c r="Q13" s="6" t="inlineStr"/>
-      <c r="R13" s="6" t="inlineStr"/>
-      <c r="S13" s="6" t="inlineStr"/>
-      <c r="T13" s="6" t="inlineStr"/>
-      <c r="U13" s="7" t="inlineStr"/>
-      <c r="V13" s="6" t="inlineStr"/>
-      <c r="W13" s="6" t="inlineStr"/>
-      <c r="X13" s="6" t="inlineStr"/>
-      <c r="Y13" s="6" t="inlineStr"/>
-      <c r="Z13" s="6" t="inlineStr"/>
-      <c r="AA13" s="6" t="inlineStr"/>
-      <c r="AB13" s="6" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
-      <c r="B14" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C14" s="6" t="inlineStr"/>
-      <c r="D14" s="6" t="inlineStr"/>
-      <c r="E14" s="6" t="inlineStr"/>
-      <c r="F14" s="6" t="inlineStr"/>
-      <c r="G14" s="6" t="inlineStr"/>
-      <c r="H14" s="7" t="inlineStr"/>
-      <c r="I14" s="6" t="inlineStr"/>
-      <c r="J14" s="6" t="inlineStr"/>
-      <c r="K14" s="6" t="inlineStr"/>
-      <c r="L14" s="6" t="inlineStr"/>
-      <c r="M14" s="6" t="inlineStr"/>
-      <c r="N14" s="6" t="inlineStr"/>
-      <c r="O14" s="7" t="inlineStr"/>
-      <c r="P14" s="6" t="inlineStr"/>
-      <c r="Q14" s="6" t="inlineStr"/>
-      <c r="R14" s="6" t="inlineStr"/>
-      <c r="S14" s="6" t="inlineStr"/>
-      <c r="T14" s="6" t="inlineStr"/>
-      <c r="U14" s="7" t="inlineStr"/>
-      <c r="V14" s="6" t="inlineStr"/>
-      <c r="W14" s="6" t="inlineStr"/>
-      <c r="X14" s="6" t="inlineStr"/>
-      <c r="Y14" s="6" t="inlineStr"/>
-      <c r="Z14" s="6" t="inlineStr"/>
-      <c r="AA14" s="6" t="inlineStr"/>
-      <c r="AB14" s="6" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="inlineStr">
-        <is>
-          <t>CP002685.1</t>
-        </is>
-      </c>
-      <c r="B15" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C15" s="6" t="inlineStr"/>
-      <c r="D15" s="6" t="inlineStr"/>
-      <c r="E15" s="6" t="inlineStr"/>
-      <c r="F15" s="6" t="inlineStr"/>
-      <c r="G15" s="6" t="inlineStr"/>
-      <c r="H15" s="7" t="inlineStr"/>
-      <c r="I15" s="6" t="inlineStr"/>
-      <c r="J15" s="6" t="inlineStr"/>
-      <c r="K15" s="6" t="inlineStr"/>
-      <c r="L15" s="6" t="inlineStr"/>
-      <c r="M15" s="6" t="inlineStr"/>
-      <c r="N15" s="6" t="inlineStr"/>
-      <c r="O15" s="7" t="inlineStr"/>
-      <c r="P15" s="6" t="inlineStr"/>
-      <c r="Q15" s="6" t="inlineStr"/>
-      <c r="R15" s="6" t="inlineStr"/>
-      <c r="S15" s="6" t="inlineStr"/>
-      <c r="T15" s="6" t="inlineStr"/>
-      <c r="U15" s="7" t="inlineStr"/>
-      <c r="V15" s="6" t="inlineStr"/>
-      <c r="W15" s="6" t="inlineStr"/>
-      <c r="X15" s="6" t="inlineStr"/>
-      <c r="Y15" s="6" t="inlineStr"/>
-      <c r="Z15" s="6" t="inlineStr"/>
-      <c r="AA15" s="6" t="inlineStr"/>
-      <c r="AB15" s="6" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="inlineStr">
-        <is>
-          <t>CP002684.1</t>
-        </is>
-      </c>
-      <c r="B16" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C16" s="6" t="inlineStr"/>
-      <c r="D16" s="6" t="inlineStr"/>
-      <c r="E16" s="6" t="inlineStr"/>
-      <c r="F16" s="6" t="inlineStr"/>
-      <c r="G16" s="6" t="inlineStr"/>
-      <c r="H16" s="7" t="inlineStr"/>
-      <c r="I16" s="6" t="inlineStr"/>
-      <c r="J16" s="6" t="inlineStr"/>
-      <c r="K16" s="6" t="inlineStr"/>
-      <c r="L16" s="6" t="inlineStr"/>
-      <c r="M16" s="6" t="inlineStr"/>
-      <c r="N16" s="6" t="inlineStr"/>
-      <c r="O16" s="7" t="inlineStr"/>
-      <c r="P16" s="6" t="inlineStr"/>
-      <c r="Q16" s="6" t="inlineStr"/>
-      <c r="R16" s="6" t="inlineStr"/>
-      <c r="S16" s="6" t="inlineStr"/>
-      <c r="T16" s="6" t="inlineStr"/>
-      <c r="U16" s="7" t="inlineStr"/>
-      <c r="V16" s="6" t="inlineStr"/>
-      <c r="W16" s="6" t="inlineStr"/>
-      <c r="X16" s="6" t="inlineStr"/>
-      <c r="Y16" s="6" t="inlineStr"/>
-      <c r="Z16" s="6" t="inlineStr"/>
-      <c r="AA16" s="6" t="inlineStr"/>
-      <c r="AB16" s="6" t="inlineStr"/>
+        <v>149890</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
implemented blast_verification to check database, updated snp_masking, but not checked
</commit_message>
<xml_diff>
--- a/ddprimer/test_data/Primers/Primers_fasta1_vs_fasta2.xlsx
+++ b/ddprimer/test_data/Primers/Primers_fasta1_vs_fasta2.xlsx
@@ -680,243 +680,241 @@
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>MTO1</t>
+          <t>PDH-E1 ALPHA</t>
         </is>
       </c>
       <c r="B3" s="7" t="inlineStr">
         <is>
-          <t>CTGGTGGATCTAGGAGGTAC</t>
+          <t>CAGTAACCTTGCCGAAGAG</t>
         </is>
       </c>
       <c r="C3" s="6" t="n">
-        <v>58.11536079407438</v>
+        <v>57.85284621491923</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>1.865360794074377</v>
+        <v>1.418635688603434</v>
       </c>
       <c r="E3" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>0.3</v>
+        <v>1.1</v>
       </c>
       <c r="H3" s="7" t="inlineStr">
         <is>
-          <t>GGGATCAGGGAGAAGATAGG</t>
+          <t>GCTCCTTACCAAGTCTGAC</t>
         </is>
       </c>
       <c r="I3" s="6" t="n">
-        <v>58.1693460818891</v>
+        <v>57.15171809660262</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>1.919346081889103</v>
+        <v>1.414071377081587</v>
       </c>
       <c r="K3" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L3" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="M3" s="6" t="n">
-        <v>1.1</v>
+        <v>3.7</v>
       </c>
       <c r="N3" s="6" t="n">
-        <v>3.784706875963479</v>
+        <v>2.832707065685021</v>
       </c>
       <c r="O3" s="7" t="inlineStr">
         <is>
-          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
+          <t>CCGTGACCATGTCCATGCCCTCAGCA</t>
         </is>
       </c>
       <c r="P3" s="6" t="n">
-        <v>64.81452393084095</v>
+        <v>64.46575342767647</v>
       </c>
       <c r="Q3" s="6" t="n">
-        <v>7.185476069159051</v>
+        <v>6.534246572323525</v>
       </c>
       <c r="R3" s="6" t="n">
-        <v>0</v>
+        <v>-0.8420321941375732</v>
       </c>
       <c r="S3" s="6" t="n">
-        <v>5.4e-07</v>
+        <v>1.51e-06</v>
       </c>
       <c r="T3" s="6" t="n">
-        <v>0.51</v>
+        <v>1.4</v>
       </c>
       <c r="U3" s="7" t="inlineStr">
         <is>
-          <t>CTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGATCCCC</t>
+          <t>CAGTAACCTTGCCGAAGAGCTCGCTCATAACAGCACGAGCAGAGACACCTTTGCTGAGGGCATGGACATGGTCACGGTAGGTACTAACGACAGAGTCAGACTTGGTAAGGAGCT</t>
         </is>
       </c>
       <c r="V3" s="6" t="n">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="W3" s="6" t="n">
-        <v>52.29357798165137</v>
+        <v>52.63157894736842</v>
       </c>
       <c r="X3" s="6" t="n">
-        <v>-3.461651563644409</v>
+        <v>-8.800433158874512</v>
       </c>
       <c r="Y3" s="6" t="inlineStr">
         <is>
-          <t>CP002686.1</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="Z3" s="6" t="inlineStr">
         <is>
-          <t>41300</t>
+          <t>48586</t>
         </is>
       </c>
       <c r="AA3" s="6" t="inlineStr">
         <is>
-          <t>LR699772.1</t>
+          <t>LR699770.1</t>
         </is>
       </c>
       <c r="AB3" s="6" t="n">
-        <v>32887</v>
+        <v>47493</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>MTO1</t>
+          <t>PDH-E1 ALPHA</t>
         </is>
       </c>
       <c r="B4" s="7" t="inlineStr">
         <is>
-          <t>CTGAATCTGGTGGATCTAGG</t>
+          <t>CGAAGAGCTCGCTCATAAC</t>
         </is>
       </c>
       <c r="C4" s="6" t="n">
-        <v>56.59552606387956</v>
+        <v>58.11854570998298</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>2.154473936120439</v>
+        <v>1.684335183667191</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>0</v>
+        <v>-0.8030736446380615</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="G4" s="6" t="n">
         <v>1.1</v>
       </c>
       <c r="H4" s="7" t="inlineStr">
         <is>
-          <t>CAGGGAGAAGATAGGTAGTG</t>
+          <t>ACCAAGTCTGACTCTGTCG</t>
         </is>
       </c>
       <c r="I4" s="6" t="n">
-        <v>55.9357109944566</v>
+        <v>58.65308273860558</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>2.814289005543401</v>
+        <v>2.218872212289785</v>
       </c>
       <c r="K4" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="M4" s="6" t="n">
         <v>3.7</v>
       </c>
       <c r="N4" s="6" t="n">
-        <v>4.96876294166384</v>
+        <v>3.903207395956976</v>
       </c>
       <c r="O4" s="7" t="inlineStr">
         <is>
-          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
+          <t>CCGTGACCATGTCCATGCCCTCAGCA</t>
         </is>
       </c>
       <c r="P4" s="6" t="n">
-        <v>64.81452393084095</v>
+        <v>64.46575342767647</v>
       </c>
       <c r="Q4" s="6" t="n">
-        <v>7.185476069159051</v>
+        <v>6.534246572323525</v>
       </c>
       <c r="R4" s="6" t="n">
-        <v>0</v>
+        <v>-0.8420321941375732</v>
       </c>
       <c r="S4" s="6" t="n">
-        <v>5.4e-07</v>
+        <v>1.51e-06</v>
       </c>
       <c r="T4" s="6" t="n">
-        <v>0.51</v>
+        <v>1.4</v>
       </c>
       <c r="U4" s="7" t="inlineStr">
         <is>
-          <t>CTGAATCTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGA</t>
+          <t>CGAAGAGCTCGCTCATAACAGCACGAGCAGAGACACCTTTGCTGAGGGCATGGACATGGTCACGGTAGGTACTAACGACAGAGTCAGACTTGGTA</t>
         </is>
       </c>
       <c r="V4" s="6" t="n">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="W4" s="6" t="n">
-        <v>50</v>
+        <v>52.63157894736842</v>
       </c>
       <c r="X4" s="6" t="n">
-        <v>-3.461651563644409</v>
+        <v>-8.800433158874512</v>
       </c>
       <c r="Y4" s="6" t="inlineStr">
         <is>
-          <t>CP002686.1</t>
+          <t>CP002684.1</t>
         </is>
       </c>
       <c r="Z4" s="6" t="inlineStr">
         <is>
-          <t>41294</t>
+          <t>48598</t>
         </is>
       </c>
       <c r="AA4" s="6" t="inlineStr">
         <is>
-          <t>LR699772.1</t>
+          <t>LR699770.1</t>
         </is>
       </c>
       <c r="AB4" s="6" t="n">
-        <v>32881</v>
+        <v>47505</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>PDH-E1 ALPHA</t>
+          <t>CYP703A2</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>CAGTAACCTTGCCGAAGAG</t>
+          <t>GAACGATCCCGATACCATC</t>
         </is>
       </c>
       <c r="C5" s="6" t="n">
-        <v>57.85284621491923</v>
+        <v>57.18013716608459</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>1.418635688603434</v>
+        <v>1.385652307599617</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>0</v>
+        <v>-0.8097348213195801</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>0.007</v>
       </c>
-      <c r="G5" s="6" t="n">
-        <v>1.1</v>
-      </c>
+      <c r="G5" s="6" t="inlineStr"/>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>GCTCCTTACCAAGTCTGAC</t>
+          <t>CACATCCATACGCTAGGTG</t>
         </is>
       </c>
       <c r="I5" s="6" t="n">
-        <v>57.15171809660262</v>
+        <v>57.40147050241876</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>1.414071377081587</v>
+        <v>1.164318971265448</v>
       </c>
       <c r="K5" s="6" t="n">
         <v>0</v>
@@ -928,21 +926,21 @@
         <v>3.7</v>
       </c>
       <c r="N5" s="6" t="n">
-        <v>2.832707065685021</v>
+        <v>2.549971278865065</v>
       </c>
       <c r="O5" s="7" t="inlineStr">
         <is>
-          <t>CCGTGACCATGTCCATGCCCTCAGCA</t>
+          <t>TCGAGACCCAAAACACTCGCCGCAGT</t>
         </is>
       </c>
       <c r="P5" s="6" t="n">
-        <v>64.46575342767647</v>
+        <v>64.30135325099201</v>
       </c>
       <c r="Q5" s="6" t="n">
-        <v>6.534246572323525</v>
+        <v>6.698646749007992</v>
       </c>
       <c r="R5" s="6" t="n">
-        <v>-0.8420321941375732</v>
+        <v>-1.419864654541016</v>
       </c>
       <c r="S5" s="6" t="n">
         <v>1.51e-06</v>
@@ -952,17 +950,17 @@
       </c>
       <c r="U5" s="7" t="inlineStr">
         <is>
-          <t>CAGTAACCTTGCCGAAGAGCTCGCTCATAACAGCACGAGCAGAGACACCTTTGCTGAGGGCATGGACATGGTCACGGTAGGTACTAACGACAGAGTCAGACTTGGTAAGGAGCT</t>
+          <t>GAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATGTGG</t>
         </is>
       </c>
       <c r="V5" s="6" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="W5" s="6" t="n">
-        <v>52.63157894736842</v>
+        <v>51.9607843137255</v>
       </c>
       <c r="X5" s="6" t="n">
-        <v>-8.800433158874512</v>
+        <v>-5.947404861450195</v>
       </c>
       <c r="Y5" s="6" t="inlineStr">
         <is>
@@ -971,7 +969,7 @@
       </c>
       <c r="Z5" s="6" t="inlineStr">
         <is>
-          <t>48586</t>
+          <t>112527</t>
         </is>
       </c>
       <c r="AA5" s="6" t="inlineStr">
@@ -980,45 +978,45 @@
         </is>
       </c>
       <c r="AB5" s="6" t="n">
-        <v>47493</v>
+        <v>111452</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>PDH-E1 ALPHA</t>
+          <t>CYP703A2</t>
         </is>
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>CGAAGAGCTCGCTCATAAC</t>
+          <t>CAACGAACGATCCCGATAC</t>
         </is>
       </c>
       <c r="C6" s="6" t="n">
-        <v>58.11854570998298</v>
+        <v>58.1158368244387</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>1.684335183667191</v>
+        <v>1.681626298122911</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>-0.8030736446380615</v>
+        <v>-0.8097348213195801</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>0.007</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>1.1</v>
+        <v>3.7</v>
       </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
-          <t>ACCAAGTCTGACTCTGTCG</t>
+          <t>ATCCATACGCTAGGTGGAC</t>
         </is>
       </c>
       <c r="I6" s="6" t="n">
-        <v>58.65308273860558</v>
+        <v>58.25082796726878</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v>2.218872212289785</v>
+        <v>1.816617440952985</v>
       </c>
       <c r="K6" s="6" t="n">
         <v>0</v>
@@ -1027,44 +1025,44 @@
         <v>0.007</v>
       </c>
       <c r="M6" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="N6" s="6" t="n">
-        <v>3.903207395956976</v>
+        <v>3.498243739075896</v>
       </c>
       <c r="O6" s="7" t="inlineStr">
         <is>
-          <t>CCGTGACCATGTCCATGCCCTCAGCA</t>
+          <t>TCATCGAGACCCAAAACACTCGCCGCA</t>
         </is>
       </c>
       <c r="P6" s="6" t="n">
-        <v>64.46575342767647</v>
+        <v>64.20487603053124</v>
       </c>
       <c r="Q6" s="6" t="n">
-        <v>6.534246572323525</v>
+        <v>7.795123969468762</v>
       </c>
       <c r="R6" s="6" t="n">
-        <v>-0.8420321941375732</v>
+        <v>-1.419864654541016</v>
       </c>
       <c r="S6" s="6" t="n">
-        <v>1.51e-06</v>
+        <v>5.4e-07</v>
       </c>
       <c r="T6" s="6" t="n">
-        <v>1.4</v>
+        <v>0.042</v>
       </c>
       <c r="U6" s="7" t="inlineStr">
         <is>
-          <t>CGAAGAGCTCGCTCATAACAGCACGAGCAGAGACACCTTTGCTGAGGGCATGGACATGGTCACGGTAGGTACTAACGACAGAGTCAGACTTGGTA</t>
+          <t>CAACGAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATG</t>
         </is>
       </c>
       <c r="V6" s="6" t="n">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="W6" s="6" t="n">
-        <v>52.63157894736842</v>
+        <v>51.45631067961165</v>
       </c>
       <c r="X6" s="6" t="n">
-        <v>-8.800433158874512</v>
+        <v>-5.947404861450195</v>
       </c>
       <c r="Y6" s="6" t="inlineStr">
         <is>
@@ -1073,7 +1071,7 @@
       </c>
       <c r="Z6" s="6" t="inlineStr">
         <is>
-          <t>48598</t>
+          <t>112523</t>
         </is>
       </c>
       <c r="AA6" s="6" t="inlineStr">
@@ -1082,209 +1080,211 @@
         </is>
       </c>
       <c r="AB6" s="6" t="n">
-        <v>47505</v>
+        <v>111448</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>CYP703A2</t>
+          <t>MTO1</t>
         </is>
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>GAACGATCCCGATACCATC</t>
+          <t>CTGGTGGATCTAGGAGGTAC</t>
         </is>
       </c>
       <c r="C7" s="6" t="n">
-        <v>57.18013716608459</v>
+        <v>58.11536079407438</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>1.385652307599617</v>
+        <v>1.865360794074377</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="G7" s="6" t="inlineStr"/>
+        <v>0.002</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>0.3</v>
+      </c>
       <c r="H7" s="7" t="inlineStr">
         <is>
-          <t>CACATCCATACGCTAGGTG</t>
+          <t>GGGATCAGGGAGAAGATAGG</t>
         </is>
       </c>
       <c r="I7" s="6" t="n">
-        <v>57.40147050241876</v>
+        <v>58.1693460818891</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>1.164318971265448</v>
+        <v>1.919346081889103</v>
       </c>
       <c r="K7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="N7" s="6" t="n">
-        <v>2.549971278865065</v>
+        <v>3.784706875963479</v>
       </c>
       <c r="O7" s="7" t="inlineStr">
         <is>
-          <t>TCGAGACCCAAAACACTCGCCGCAGT</t>
+          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
         </is>
       </c>
       <c r="P7" s="6" t="n">
-        <v>64.30135325099201</v>
+        <v>64.81452393084095</v>
       </c>
       <c r="Q7" s="6" t="n">
-        <v>6.698646749007992</v>
+        <v>7.185476069159051</v>
       </c>
       <c r="R7" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>0</v>
       </c>
       <c r="S7" s="6" t="n">
-        <v>1.51e-06</v>
+        <v>5.4e-07</v>
       </c>
       <c r="T7" s="6" t="n">
-        <v>1.4</v>
+        <v>0.51</v>
       </c>
       <c r="U7" s="7" t="inlineStr">
         <is>
-          <t>GAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATGTGG</t>
+          <t>CTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGATCCCC</t>
         </is>
       </c>
       <c r="V7" s="6" t="n">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="W7" s="6" t="n">
-        <v>51.9607843137255</v>
+        <v>52.29357798165137</v>
       </c>
       <c r="X7" s="6" t="n">
-        <v>-5.947404861450195</v>
+        <v>-3.461651563644409</v>
       </c>
       <c r="Y7" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>CP002686.1</t>
         </is>
       </c>
       <c r="Z7" s="6" t="inlineStr">
         <is>
-          <t>112527</t>
+          <t>41300</t>
         </is>
       </c>
       <c r="AA7" s="6" t="inlineStr">
         <is>
-          <t>LR699770.1</t>
+          <t>LR699772.1</t>
         </is>
       </c>
       <c r="AB7" s="6" t="n">
-        <v>111452</v>
+        <v>32887</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>CYP703A2</t>
+          <t>MTO1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>CAACGAACGATCCCGATAC</t>
+          <t>CTGAATCTGGTGGATCTAGG</t>
         </is>
       </c>
       <c r="C8" s="6" t="n">
-        <v>58.1158368244387</v>
+        <v>56.59552606387956</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>1.681626298122911</v>
+        <v>2.154473936120439</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="H8" s="7" t="inlineStr">
         <is>
-          <t>ATCCATACGCTAGGTGGAC</t>
+          <t>CAGGGAGAAGATAGGTAGTG</t>
         </is>
       </c>
       <c r="I8" s="6" t="n">
-        <v>58.25082796726878</v>
+        <v>55.9357109944566</v>
       </c>
       <c r="J8" s="6" t="n">
-        <v>1.816617440952985</v>
+        <v>2.814289005543401</v>
       </c>
       <c r="K8" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L8" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v>1.1</v>
+        <v>3.7</v>
       </c>
       <c r="N8" s="6" t="n">
-        <v>3.498243739075896</v>
+        <v>4.96876294166384</v>
       </c>
       <c r="O8" s="7" t="inlineStr">
         <is>
-          <t>TCATCGAGACCCAAAACACTCGCCGCA</t>
+          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
         </is>
       </c>
       <c r="P8" s="6" t="n">
-        <v>64.20487603053124</v>
+        <v>64.81452393084095</v>
       </c>
       <c r="Q8" s="6" t="n">
-        <v>7.795123969468762</v>
+        <v>7.185476069159051</v>
       </c>
       <c r="R8" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>0</v>
       </c>
       <c r="S8" s="6" t="n">
         <v>5.4e-07</v>
       </c>
       <c r="T8" s="6" t="n">
-        <v>0.042</v>
+        <v>0.51</v>
       </c>
       <c r="U8" s="7" t="inlineStr">
         <is>
-          <t>CAACGAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATG</t>
+          <t>CTGAATCTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGA</t>
         </is>
       </c>
       <c r="V8" s="6" t="n">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="W8" s="6" t="n">
-        <v>51.45631067961165</v>
+        <v>50</v>
       </c>
       <c r="X8" s="6" t="n">
-        <v>-5.947404861450195</v>
+        <v>-3.461651563644409</v>
       </c>
       <c r="Y8" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>CP002686.1</t>
         </is>
       </c>
       <c r="Z8" s="6" t="inlineStr">
         <is>
-          <t>112523</t>
+          <t>41294</t>
         </is>
       </c>
       <c r="AA8" s="6" t="inlineStr">
         <is>
-          <t>LR699770.1</t>
+          <t>LR699772.1</t>
         </is>
       </c>
       <c r="AB8" s="6" t="n">
-        <v>111448</v>
+        <v>32881</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
adjusted script folder structure
</commit_message>
<xml_diff>
--- a/ddprimer/test_data/Primers/Primers_fasta1_vs_fasta2.xlsx
+++ b/ddprimer/test_data/Primers/Primers_fasta1_vs_fasta2.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -680,241 +680,243 @@
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>PDH-E1 ALPHA</t>
+          <t>MTO1</t>
         </is>
       </c>
       <c r="B3" s="7" t="inlineStr">
         <is>
-          <t>CAGTAACCTTGCCGAAGAG</t>
+          <t>CTGGTGGATCTAGGAGGTAC</t>
         </is>
       </c>
       <c r="C3" s="6" t="n">
-        <v>57.85284621491923</v>
+        <v>58.11536079407438</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>1.418635688603434</v>
+        <v>1.865360794074377</v>
       </c>
       <c r="E3" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>1.1</v>
+        <v>0.3</v>
       </c>
       <c r="H3" s="7" t="inlineStr">
         <is>
-          <t>GCTCCTTACCAAGTCTGAC</t>
+          <t>GGGATCAGGGAGAAGATAGG</t>
         </is>
       </c>
       <c r="I3" s="6" t="n">
-        <v>57.15171809660262</v>
+        <v>58.1693460818891</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>1.414071377081587</v>
+        <v>1.919346081889103</v>
       </c>
       <c r="K3" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L3" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="M3" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="N3" s="6" t="n">
-        <v>2.832707065685021</v>
+        <v>3.784706875963479</v>
       </c>
       <c r="O3" s="7" t="inlineStr">
         <is>
-          <t>CCGTGACCATGTCCATGCCCTCAGCA</t>
+          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
         </is>
       </c>
       <c r="P3" s="6" t="n">
-        <v>64.46575342767647</v>
+        <v>64.81452393084095</v>
       </c>
       <c r="Q3" s="6" t="n">
-        <v>6.534246572323525</v>
+        <v>7.185476069159051</v>
       </c>
       <c r="R3" s="6" t="n">
-        <v>-0.8420321941375732</v>
+        <v>0</v>
       </c>
       <c r="S3" s="6" t="n">
-        <v>1.51e-06</v>
+        <v>5.4e-07</v>
       </c>
       <c r="T3" s="6" t="n">
-        <v>1.4</v>
+        <v>0.51</v>
       </c>
       <c r="U3" s="7" t="inlineStr">
         <is>
-          <t>CAGTAACCTTGCCGAAGAGCTCGCTCATAACAGCACGAGCAGAGACACCTTTGCTGAGGGCATGGACATGGTCACGGTAGGTACTAACGACAGAGTCAGACTTGGTAAGGAGCT</t>
+          <t>CTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGATCCCC</t>
         </is>
       </c>
       <c r="V3" s="6" t="n">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="W3" s="6" t="n">
-        <v>52.63157894736842</v>
+        <v>52.29357798165137</v>
       </c>
       <c r="X3" s="6" t="n">
-        <v>-8.800433158874512</v>
+        <v>-3.461651563644409</v>
       </c>
       <c r="Y3" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>CP002686.1</t>
         </is>
       </c>
       <c r="Z3" s="6" t="inlineStr">
         <is>
-          <t>48586</t>
+          <t>41300</t>
         </is>
       </c>
       <c r="AA3" s="6" t="inlineStr">
         <is>
-          <t>LR699770.1</t>
+          <t>LR699772.1</t>
         </is>
       </c>
       <c r="AB3" s="6" t="n">
-        <v>47493</v>
+        <v>32887</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>PDH-E1 ALPHA</t>
+          <t>MTO1</t>
         </is>
       </c>
       <c r="B4" s="7" t="inlineStr">
         <is>
-          <t>CGAAGAGCTCGCTCATAAC</t>
+          <t>CTGAATCTGGTGGATCTAGG</t>
         </is>
       </c>
       <c r="C4" s="6" t="n">
-        <v>58.11854570998298</v>
+        <v>56.59552606387956</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>1.684335183667191</v>
+        <v>2.154473936120439</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>-0.8030736446380615</v>
+        <v>0</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="G4" s="6" t="n">
         <v>1.1</v>
       </c>
       <c r="H4" s="7" t="inlineStr">
         <is>
-          <t>ACCAAGTCTGACTCTGTCG</t>
+          <t>CAGGGAGAAGATAGGTAGTG</t>
         </is>
       </c>
       <c r="I4" s="6" t="n">
-        <v>58.65308273860558</v>
+        <v>55.9357109944566</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>2.218872212289785</v>
+        <v>2.814289005543401</v>
       </c>
       <c r="K4" s="6" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="M4" s="6" t="n">
         <v>3.7</v>
       </c>
       <c r="N4" s="6" t="n">
-        <v>3.903207395956976</v>
+        <v>4.96876294166384</v>
       </c>
       <c r="O4" s="7" t="inlineStr">
         <is>
-          <t>CCGTGACCATGTCCATGCCCTCAGCA</t>
+          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
         </is>
       </c>
       <c r="P4" s="6" t="n">
-        <v>64.46575342767647</v>
+        <v>64.81452393084095</v>
       </c>
       <c r="Q4" s="6" t="n">
-        <v>6.534246572323525</v>
+        <v>7.185476069159051</v>
       </c>
       <c r="R4" s="6" t="n">
-        <v>-0.8420321941375732</v>
+        <v>0</v>
       </c>
       <c r="S4" s="6" t="n">
-        <v>1.51e-06</v>
+        <v>5.4e-07</v>
       </c>
       <c r="T4" s="6" t="n">
-        <v>1.4</v>
+        <v>0.51</v>
       </c>
       <c r="U4" s="7" t="inlineStr">
         <is>
-          <t>CGAAGAGCTCGCTCATAACAGCACGAGCAGAGACACCTTTGCTGAGGGCATGGACATGGTCACGGTAGGTACTAACGACAGAGTCAGACTTGGTA</t>
+          <t>CTGAATCTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGA</t>
         </is>
       </c>
       <c r="V4" s="6" t="n">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="W4" s="6" t="n">
-        <v>52.63157894736842</v>
+        <v>50</v>
       </c>
       <c r="X4" s="6" t="n">
-        <v>-8.800433158874512</v>
+        <v>-3.461651563644409</v>
       </c>
       <c r="Y4" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>CP002686.1</t>
         </is>
       </c>
       <c r="Z4" s="6" t="inlineStr">
         <is>
-          <t>48598</t>
+          <t>41294</t>
         </is>
       </c>
       <c r="AA4" s="6" t="inlineStr">
         <is>
-          <t>LR699770.1</t>
+          <t>LR699772.1</t>
         </is>
       </c>
       <c r="AB4" s="6" t="n">
-        <v>47505</v>
+        <v>32881</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>CYP703A2</t>
+          <t>XSP1</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>GAACGATCCCGATACCATC</t>
+          <t>CTACGACATGGACGACATC</t>
         </is>
       </c>
       <c r="C5" s="6" t="n">
-        <v>57.18013716608459</v>
+        <v>57.44369071181501</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>1.385652307599617</v>
+        <v>1.1220987618692</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>-0.3097348213195801</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>0.007</v>
       </c>
-      <c r="G5" s="6" t="inlineStr"/>
+      <c r="G5" s="6" t="n">
+        <v>1.1</v>
+      </c>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>CACATCCATACGCTAGGTG</t>
+          <t>GACAATGGAGGAACAGCTC</t>
         </is>
       </c>
       <c r="I5" s="6" t="n">
-        <v>57.40147050241876</v>
+        <v>57.83082272420569</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>1.164318971265448</v>
+        <v>1.396612197889898</v>
       </c>
       <c r="K5" s="6" t="n">
         <v>0</v>
@@ -923,24 +925,24 @@
         <v>0.007</v>
       </c>
       <c r="M5" s="6" t="n">
-        <v>3.7</v>
+        <v>1.1</v>
       </c>
       <c r="N5" s="6" t="n">
-        <v>2.549971278865065</v>
+        <v>2.518710959759098</v>
       </c>
       <c r="O5" s="7" t="inlineStr">
         <is>
-          <t>TCGAGACCCAAAACACTCGCCGCAGT</t>
+          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
         </is>
       </c>
       <c r="P5" s="6" t="n">
-        <v>64.30135325099201</v>
+        <v>64.22598535419934</v>
       </c>
       <c r="Q5" s="6" t="n">
-        <v>6.698646749007992</v>
+        <v>6.774014645800662</v>
       </c>
       <c r="R5" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>-0.7341697216033936</v>
       </c>
       <c r="S5" s="6" t="n">
         <v>1.51e-06</v>
@@ -950,73 +952,73 @@
       </c>
       <c r="U5" s="7" t="inlineStr">
         <is>
-          <t>GAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATGTGG</t>
+          <t>CTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCC</t>
         </is>
       </c>
       <c r="V5" s="6" t="n">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="W5" s="6" t="n">
-        <v>51.9607843137255</v>
+        <v>53.98230088495575</v>
       </c>
       <c r="X5" s="6" t="n">
-        <v>-5.947404861450195</v>
+        <v>-6.521465301513672</v>
       </c>
       <c r="Y5" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>CP002687.1</t>
         </is>
       </c>
       <c r="Z5" s="6" t="inlineStr">
         <is>
-          <t>112527</t>
+          <t>96840</t>
         </is>
       </c>
       <c r="AA5" s="6" t="inlineStr">
         <is>
-          <t>LR699770.1</t>
+          <t>LR699773.1</t>
         </is>
       </c>
       <c r="AB5" s="6" t="n">
-        <v>111452</v>
+        <v>149749</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>CYP703A2</t>
+          <t>XSP1</t>
         </is>
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>CAACGAACGATCCCGATAC</t>
+          <t>CTGGCTTAGTCTACGACATG</t>
         </is>
       </c>
       <c r="C6" s="6" t="n">
-        <v>58.1158368244387</v>
+        <v>57.6139686963578</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>1.681626298122911</v>
+        <v>1.363968696357801</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="G6" s="6" t="n">
         <v>3.7</v>
       </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
-          <t>ATCCATACGCTAGGTGGAC</t>
+          <t>AGGGACAATGGAGGAACAG</t>
         </is>
       </c>
       <c r="I6" s="6" t="n">
-        <v>58.25082796726878</v>
+        <v>58.60725372965351</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v>1.816617440952985</v>
+        <v>2.173043203337716</v>
       </c>
       <c r="K6" s="6" t="n">
         <v>0</v>
@@ -1028,97 +1030,97 @@
         <v>1.1</v>
       </c>
       <c r="N6" s="6" t="n">
-        <v>3.498243739075896</v>
+        <v>3.537011899695518</v>
       </c>
       <c r="O6" s="7" t="inlineStr">
         <is>
-          <t>TCATCGAGACCCAAAACACTCGCCGCA</t>
+          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
         </is>
       </c>
       <c r="P6" s="6" t="n">
-        <v>64.20487603053124</v>
+        <v>64.22598535419934</v>
       </c>
       <c r="Q6" s="6" t="n">
-        <v>7.795123969468762</v>
+        <v>6.774014645800662</v>
       </c>
       <c r="R6" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>-0.7341697216033936</v>
       </c>
       <c r="S6" s="6" t="n">
-        <v>5.4e-07</v>
+        <v>1.51e-06</v>
       </c>
       <c r="T6" s="6" t="n">
-        <v>0.042</v>
+        <v>1.4</v>
       </c>
       <c r="U6" s="7" t="inlineStr">
         <is>
-          <t>CAACGAACGATCCCGATACCATCCGTGAGATTCTTTTGCGGCAGGACGATGTTTTTTCATCGAGACCCAAAACACTCGCCGCAGTCCACCTAGCGTATGGATG</t>
+          <t>CTGGCTTAGTCTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCCCTG</t>
         </is>
       </c>
       <c r="V6" s="6" t="n">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="W6" s="6" t="n">
-        <v>51.45631067961165</v>
+        <v>53.96825396825397</v>
       </c>
       <c r="X6" s="6" t="n">
-        <v>-5.947404861450195</v>
+        <v>-6.521465301513672</v>
       </c>
       <c r="Y6" s="6" t="inlineStr">
         <is>
-          <t>CP002684.1</t>
+          <t>CP002687.1</t>
         </is>
       </c>
       <c r="Z6" s="6" t="inlineStr">
         <is>
-          <t>112523</t>
+          <t>96830</t>
         </is>
       </c>
       <c r="AA6" s="6" t="inlineStr">
         <is>
-          <t>LR699770.1</t>
+          <t>LR699773.1</t>
         </is>
       </c>
       <c r="AB6" s="6" t="n">
-        <v>111448</v>
+        <v>149739</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>MTO1</t>
+          <t>XSP1</t>
         </is>
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>CTGGTGGATCTAGGAGGTAC</t>
+          <t>CCCAACAATCCAACTCACG</t>
         </is>
       </c>
       <c r="C7" s="6" t="n">
-        <v>58.11536079407438</v>
+        <v>58.74250943646473</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>1.865360794074377</v>
+        <v>2.308298910148938</v>
       </c>
       <c r="E7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>0.3</v>
+        <v>3.7</v>
       </c>
       <c r="H7" s="7" t="inlineStr">
         <is>
-          <t>GGGATCAGGGAGAAGATAGG</t>
+          <t>CCACCACTTTGAAGCTTCTC</t>
         </is>
       </c>
       <c r="I7" s="6" t="n">
-        <v>58.1693460818891</v>
+        <v>58.87532172899461</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>1.919346081889103</v>
+        <v>2.625321728994606</v>
       </c>
       <c r="K7" s="6" t="n">
         <v>0</v>
@@ -1127,469 +1129,61 @@
         <v>0.002</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v>1.1</v>
+        <v>0.3</v>
       </c>
       <c r="N7" s="6" t="n">
-        <v>3.784706875963479</v>
+        <v>4.933620639143545</v>
       </c>
       <c r="O7" s="7" t="inlineStr">
         <is>
-          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
+          <t>CCGCCACCGTCCGAGCACCG</t>
         </is>
       </c>
       <c r="P7" s="6" t="n">
-        <v>64.81452393084095</v>
+        <v>64.7335341111355</v>
       </c>
       <c r="Q7" s="6" t="n">
-        <v>7.185476069159051</v>
+        <v>0.2664658888645022</v>
       </c>
       <c r="R7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="S7" s="6" t="n">
-        <v>5.4e-07</v>
+        <v>0.002</v>
       </c>
       <c r="T7" s="6" t="n">
-        <v>0.51</v>
+        <v>1.1</v>
       </c>
       <c r="U7" s="7" t="inlineStr">
         <is>
-          <t>CTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGATCCCC</t>
+          <t>CCCAACAATCCAACTCACGTTGAGATCCGCCAAAACGTCCACATTGGCTGTGTTCAGGCGGAGAGTCACCAACGTGGGACCACCGTCGTCGGTCTACACCGCCACCGTCCGAGCACCGAAAGGAGTAGAAATCACGGTGGAGCCACAGAGTTTGTCATTTTCAAAGGCTTCACAAAAGAGAAGCTTCAAAGTGGTGGT</t>
         </is>
       </c>
       <c r="V7" s="6" t="n">
-        <v>108</v>
+        <v>197</v>
       </c>
       <c r="W7" s="6" t="n">
-        <v>52.29357798165137</v>
+        <v>53.03030303030303</v>
       </c>
       <c r="X7" s="6" t="n">
-        <v>-3.461651563644409</v>
+        <v>-17.26604652404785</v>
       </c>
       <c r="Y7" s="6" t="inlineStr">
         <is>
-          <t>CP002686.1</t>
+          <t>CP002687.1</t>
         </is>
       </c>
       <c r="Z7" s="6" t="inlineStr">
         <is>
-          <t>41300</t>
+          <t>96981</t>
         </is>
       </c>
       <c r="AA7" s="6" t="inlineStr">
         <is>
-          <t>LR699772.1</t>
+          <t>LR699773.1</t>
         </is>
       </c>
       <c r="AB7" s="6" t="n">
-        <v>32887</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="inlineStr">
-        <is>
-          <t>MTO1</t>
-        </is>
-      </c>
-      <c r="B8" s="7" t="inlineStr">
-        <is>
-          <t>CTGAATCTGGTGGATCTAGG</t>
-        </is>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>56.59552606387956</v>
-      </c>
-      <c r="D8" s="6" t="n">
-        <v>2.154473936120439</v>
-      </c>
-      <c r="E8" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="G8" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="H8" s="7" t="inlineStr">
-        <is>
-          <t>CAGGGAGAAGATAGGTAGTG</t>
-        </is>
-      </c>
-      <c r="I8" s="6" t="n">
-        <v>55.9357109944566</v>
-      </c>
-      <c r="J8" s="6" t="n">
-        <v>2.814289005543401</v>
-      </c>
-      <c r="K8" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="M8" s="6" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="N8" s="6" t="n">
-        <v>4.96876294166384</v>
-      </c>
-      <c r="O8" s="7" t="inlineStr">
-        <is>
-          <t>CCGATGGGAGCCTCACTGTTCATGCCG</t>
-        </is>
-      </c>
-      <c r="P8" s="6" t="n">
-        <v>64.81452393084095</v>
-      </c>
-      <c r="Q8" s="6" t="n">
-        <v>7.185476069159051</v>
-      </c>
-      <c r="R8" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" s="6" t="n">
-        <v>5.4e-07</v>
-      </c>
-      <c r="T8" s="6" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="U8" s="7" t="inlineStr">
-        <is>
-          <t>CTGAATCTGGTGGATCTAGGAGGTACCGGCATGAACAGTGAGGCTCCCATCGGAGCTCAAGAAAGAATGTTTGGAATCCGTCAGCTGTACACTACCTATCTTCTCCCTGA</t>
-        </is>
-      </c>
-      <c r="V8" s="6" t="n">
-        <v>109</v>
-      </c>
-      <c r="W8" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="X8" s="6" t="n">
-        <v>-3.461651563644409</v>
-      </c>
-      <c r="Y8" s="6" t="inlineStr">
-        <is>
-          <t>CP002686.1</t>
-        </is>
-      </c>
-      <c r="Z8" s="6" t="inlineStr">
-        <is>
-          <t>41294</t>
-        </is>
-      </c>
-      <c r="AA8" s="6" t="inlineStr">
-        <is>
-          <t>LR699772.1</t>
-        </is>
-      </c>
-      <c r="AB8" s="6" t="n">
-        <v>32881</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>XSP1</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>CTACGACATGGACGACATC</t>
-        </is>
-      </c>
-      <c r="C9" s="6" t="n">
-        <v>57.44369071181501</v>
-      </c>
-      <c r="D9" s="6" t="n">
-        <v>1.1220987618692</v>
-      </c>
-      <c r="E9" s="6" t="n">
-        <v>-0.3097348213195801</v>
-      </c>
-      <c r="F9" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="G9" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="H9" s="7" t="inlineStr">
-        <is>
-          <t>GACAATGGAGGAACAGCTC</t>
-        </is>
-      </c>
-      <c r="I9" s="6" t="n">
-        <v>57.83082272420569</v>
-      </c>
-      <c r="J9" s="6" t="n">
-        <v>1.396612197889898</v>
-      </c>
-      <c r="K9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="M9" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="N9" s="6" t="n">
-        <v>2.518710959759098</v>
-      </c>
-      <c r="O9" s="7" t="inlineStr">
-        <is>
-          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
-        </is>
-      </c>
-      <c r="P9" s="6" t="n">
-        <v>64.22598535419934</v>
-      </c>
-      <c r="Q9" s="6" t="n">
-        <v>6.774014645800662</v>
-      </c>
-      <c r="R9" s="6" t="n">
-        <v>-0.7341697216033936</v>
-      </c>
-      <c r="S9" s="6" t="n">
-        <v>1.51e-06</v>
-      </c>
-      <c r="T9" s="6" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="U9" s="7" t="inlineStr">
-        <is>
-          <t>CTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCC</t>
-        </is>
-      </c>
-      <c r="V9" s="6" t="n">
-        <v>112</v>
-      </c>
-      <c r="W9" s="6" t="n">
-        <v>53.98230088495575</v>
-      </c>
-      <c r="X9" s="6" t="n">
-        <v>-6.521465301513672</v>
-      </c>
-      <c r="Y9" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
-      <c r="Z9" s="6" t="inlineStr">
-        <is>
-          <t>96840</t>
-        </is>
-      </c>
-      <c r="AA9" s="6" t="inlineStr">
-        <is>
-          <t>LR699773.1</t>
-        </is>
-      </c>
-      <c r="AB9" s="6" t="n">
-        <v>149749</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>XSP1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>CTGGCTTAGTCTACGACATG</t>
-        </is>
-      </c>
-      <c r="C10" s="6" t="n">
-        <v>57.6139686963578</v>
-      </c>
-      <c r="D10" s="6" t="n">
-        <v>1.363968696357801</v>
-      </c>
-      <c r="E10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="G10" s="6" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="H10" s="7" t="inlineStr">
-        <is>
-          <t>AGGGACAATGGAGGAACAG</t>
-        </is>
-      </c>
-      <c r="I10" s="6" t="n">
-        <v>58.60725372965351</v>
-      </c>
-      <c r="J10" s="6" t="n">
-        <v>2.173043203337716</v>
-      </c>
-      <c r="K10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="M10" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="N10" s="6" t="n">
-        <v>3.537011899695518</v>
-      </c>
-      <c r="O10" s="7" t="inlineStr">
-        <is>
-          <t>AGCTCCATTGGTGGGTACACGCTCCG</t>
-        </is>
-      </c>
-      <c r="P10" s="6" t="n">
-        <v>64.22598535419934</v>
-      </c>
-      <c r="Q10" s="6" t="n">
-        <v>6.774014645800662</v>
-      </c>
-      <c r="R10" s="6" t="n">
-        <v>-0.7341697216033936</v>
-      </c>
-      <c r="S10" s="6" t="n">
-        <v>1.51e-06</v>
-      </c>
-      <c r="T10" s="6" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="U10" s="7" t="inlineStr">
-        <is>
-          <t>CTGGCTTAGTCTACGACATGGACGACATCTCCTATGTTCAGTTCTTGTGCGGCGAAGGCTACAACGCAACCACTCTAGCTCCATTGGTGGGTACACGCTCCGTGAGCTGTTCCTCCATTGTCCCTG</t>
-        </is>
-      </c>
-      <c r="V10" s="6" t="n">
-        <v>125</v>
-      </c>
-      <c r="W10" s="6" t="n">
-        <v>53.96825396825397</v>
-      </c>
-      <c r="X10" s="6" t="n">
-        <v>-6.521465301513672</v>
-      </c>
-      <c r="Y10" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
-      <c r="Z10" s="6" t="inlineStr">
-        <is>
-          <t>96830</t>
-        </is>
-      </c>
-      <c r="AA10" s="6" t="inlineStr">
-        <is>
-          <t>LR699773.1</t>
-        </is>
-      </c>
-      <c r="AB10" s="6" t="n">
-        <v>149739</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>XSP1</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>CCCAACAATCCAACTCACG</t>
-        </is>
-      </c>
-      <c r="C11" s="6" t="n">
-        <v>58.74250943646473</v>
-      </c>
-      <c r="D11" s="6" t="n">
-        <v>2.308298910148938</v>
-      </c>
-      <c r="E11" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="G11" s="6" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="H11" s="7" t="inlineStr">
-        <is>
-          <t>CCACCACTTTGAAGCTTCTC</t>
-        </is>
-      </c>
-      <c r="I11" s="6" t="n">
-        <v>58.87532172899461</v>
-      </c>
-      <c r="J11" s="6" t="n">
-        <v>2.625321728994606</v>
-      </c>
-      <c r="K11" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="M11" s="6" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="N11" s="6" t="n">
-        <v>4.933620639143545</v>
-      </c>
-      <c r="O11" s="7" t="inlineStr">
-        <is>
-          <t>CCGCCACCGTCCGAGCACCG</t>
-        </is>
-      </c>
-      <c r="P11" s="6" t="n">
-        <v>64.7335341111355</v>
-      </c>
-      <c r="Q11" s="6" t="n">
-        <v>0.2664658888645022</v>
-      </c>
-      <c r="R11" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S11" s="6" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="T11" s="6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="U11" s="7" t="inlineStr">
-        <is>
-          <t>CCCAACAATCCAACTCACGTTGAGATCCGCCAAAACGTCCACATTGGCTGTGTTCAGGCGGAGAGTCACCAACGTGGGACCACCGTCGTCGGTCTACACCGCCACCGTCCGAGCACCGAAAGGAGTAGAAATCACGGTGGAGCCACAGAGTTTGTCATTTTCAAAGGCTTCACAAAAGAGAAGCTTCAAAGTGGTGGT</t>
-        </is>
-      </c>
-      <c r="V11" s="6" t="n">
-        <v>197</v>
-      </c>
-      <c r="W11" s="6" t="n">
-        <v>53.03030303030303</v>
-      </c>
-      <c r="X11" s="6" t="n">
-        <v>-17.26604652404785</v>
-      </c>
-      <c r="Y11" s="6" t="inlineStr">
-        <is>
-          <t>CP002687.1</t>
-        </is>
-      </c>
-      <c r="Z11" s="6" t="inlineStr">
-        <is>
-          <t>96981</t>
-        </is>
-      </c>
-      <c r="AA11" s="6" t="inlineStr">
-        <is>
-          <t>LR699773.1</t>
-        </is>
-      </c>
-      <c r="AB11" s="6" t="n">
         <v>149890</v>
       </c>
     </row>

</xml_diff>